<commit_message>
Train all models and regenerate SSP predictions
Fix metrics bug in regression.py where RMSE/MSE/MAE/MAPE were
incorrectly taken from the last parameter combination instead of
the best one. Now properly tracks metrics for the best params.

Cubist selected as best model (CV R² = 0.6699). Regenerated
SSP2-4.5 and SSP5-8.5 predictions and analysis outputs.
</commit_message>
<xml_diff>
--- a/Pipeline/SSP2-4.5/banana_yield_analysis.xlsx
+++ b/Pipeline/SSP2-4.5/banana_yield_analysis.xlsx
@@ -671,10 +671,10 @@
         <v>7.46</v>
       </c>
       <c r="C2">
-        <v>7.23</v>
+        <v>7.29</v>
       </c>
       <c r="D2">
-        <v>-3.08</v>
+        <v>-2.24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -713,10 +713,10 @@
         <v>6.79</v>
       </c>
       <c r="C5">
-        <v>6.46</v>
+        <v>7.27</v>
       </c>
       <c r="D5">
-        <v>-4.87</v>
+        <v>7.06</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -727,10 +727,10 @@
         <v>15.86</v>
       </c>
       <c r="C6">
-        <v>11.21</v>
+        <v>10.97</v>
       </c>
       <c r="D6">
-        <v>-29.33</v>
+        <v>-30.82</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -741,10 +741,10 @@
         <v>10.96</v>
       </c>
       <c r="C7">
-        <v>10.05</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="D7">
-        <v>-8.279999999999999</v>
+        <v>-15.86</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -755,10 +755,10 @@
         <v>6.76</v>
       </c>
       <c r="C8">
-        <v>7.5</v>
+        <v>7.69</v>
       </c>
       <c r="D8">
-        <v>11.08</v>
+        <v>13.77</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -769,10 +769,10 @@
         <v>3.91</v>
       </c>
       <c r="C9">
-        <v>4.65</v>
+        <v>4.42</v>
       </c>
       <c r="D9">
-        <v>18.83</v>
+        <v>13.01</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -783,10 +783,10 @@
         <v>3.11</v>
       </c>
       <c r="C10">
-        <v>3.44</v>
+        <v>3.18</v>
       </c>
       <c r="D10">
-        <v>10.58</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -797,10 +797,10 @@
         <v>5.66</v>
       </c>
       <c r="C11">
-        <v>6.53</v>
+        <v>6.42</v>
       </c>
       <c r="D11">
-        <v>15.4</v>
+        <v>13.38</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -811,10 +811,10 @@
         <v>2.95</v>
       </c>
       <c r="C12">
-        <v>5.7</v>
+        <v>5.87</v>
       </c>
       <c r="D12">
-        <v>93.37</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -828,7 +828,7 @@
         <v>4.49</v>
       </c>
       <c r="D13">
-        <v>-22.98</v>
+        <v>-23.07</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -839,10 +839,10 @@
         <v>6.66</v>
       </c>
       <c r="C14">
-        <v>5.43</v>
+        <v>5.1</v>
       </c>
       <c r="D14">
-        <v>-18.43</v>
+        <v>-23.43</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -853,10 +853,10 @@
         <v>8.76</v>
       </c>
       <c r="C15">
-        <v>9.18</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="D15">
-        <v>4.77</v>
+        <v>5.14</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -867,10 +867,10 @@
         <v>12.01</v>
       </c>
       <c r="C16">
-        <v>14.6</v>
+        <v>14.5</v>
       </c>
       <c r="D16">
-        <v>21.58</v>
+        <v>20.75</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -881,10 +881,10 @@
         <v>61.85</v>
       </c>
       <c r="C17">
-        <v>58.54</v>
+        <v>57.66</v>
       </c>
       <c r="D17">
-        <v>-5.35</v>
+        <v>-6.77</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -895,10 +895,10 @@
         <v>13.07</v>
       </c>
       <c r="C18">
-        <v>13.53</v>
+        <v>13.1</v>
       </c>
       <c r="D18">
-        <v>3.47</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -909,10 +909,10 @@
         <v>13.86</v>
       </c>
       <c r="C19">
-        <v>11.51</v>
+        <v>11.98</v>
       </c>
       <c r="D19">
-        <v>-16.99</v>
+        <v>-13.55</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -923,10 +923,10 @@
         <v>1.88</v>
       </c>
       <c r="C20">
-        <v>2.42</v>
+        <v>2.39</v>
       </c>
       <c r="D20">
-        <v>29.12</v>
+        <v>27.29</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -940,7 +940,7 @@
         <v>3.78</v>
       </c>
       <c r="D21">
-        <v>19.15</v>
+        <v>19.26</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -965,10 +965,10 @@
         <v>6.85</v>
       </c>
       <c r="C23">
-        <v>8.550000000000001</v>
+        <v>8.23</v>
       </c>
       <c r="D23">
-        <v>24.86</v>
+        <v>20.21</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -979,10 +979,10 @@
         <v>2.64</v>
       </c>
       <c r="C24">
-        <v>3.14</v>
+        <v>3.22</v>
       </c>
       <c r="D24">
-        <v>18.86</v>
+        <v>21.91</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -993,10 +993,10 @@
         <v>5.68</v>
       </c>
       <c r="C25">
-        <v>5.65</v>
+        <v>5.46</v>
       </c>
       <c r="D25">
-        <v>-0.52</v>
+        <v>-3.92</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1007,10 +1007,10 @@
         <v>8.33</v>
       </c>
       <c r="C26">
-        <v>9.42</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="D26">
-        <v>13.12</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1021,10 +1021,10 @@
         <v>37.95</v>
       </c>
       <c r="C27">
-        <v>38.47</v>
+        <v>38.79</v>
       </c>
       <c r="D27">
-        <v>1.38</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1035,10 +1035,10 @@
         <v>15.45</v>
       </c>
       <c r="C28">
-        <v>17.01</v>
+        <v>16.95</v>
       </c>
       <c r="D28">
-        <v>10.08</v>
+        <v>9.699999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1049,10 +1049,10 @@
         <v>42</v>
       </c>
       <c r="C29">
-        <v>36.26</v>
+        <v>37.8</v>
       </c>
       <c r="D29">
-        <v>-13.66</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1063,10 +1063,10 @@
         <v>43.63</v>
       </c>
       <c r="C30">
-        <v>42.97</v>
+        <v>43.74</v>
       </c>
       <c r="D30">
-        <v>-1.52</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1077,10 +1077,10 @@
         <v>38.75</v>
       </c>
       <c r="C31">
-        <v>40.81</v>
+        <v>41.4</v>
       </c>
       <c r="D31">
-        <v>5.33</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1119,10 +1119,10 @@
         <v>11.73</v>
       </c>
       <c r="C34">
-        <v>10.3</v>
+        <v>11.8</v>
       </c>
       <c r="D34">
-        <v>-12.25</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1133,10 +1133,10 @@
         <v>7.4</v>
       </c>
       <c r="C35">
-        <v>8.06</v>
+        <v>7.83</v>
       </c>
       <c r="D35">
-        <v>8.949999999999999</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1147,10 +1147,10 @@
         <v>6.26</v>
       </c>
       <c r="C36">
-        <v>6.33</v>
+        <v>6.49</v>
       </c>
       <c r="D36">
-        <v>1.1</v>
+        <v>3.72</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1161,10 +1161,10 @@
         <v>6.67</v>
       </c>
       <c r="C37">
-        <v>7.41</v>
+        <v>7.54</v>
       </c>
       <c r="D37">
-        <v>11.18</v>
+        <v>13.09</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1175,10 +1175,10 @@
         <v>9.93</v>
       </c>
       <c r="C38">
-        <v>10.68</v>
+        <v>10.08</v>
       </c>
       <c r="D38">
-        <v>7.49</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1203,10 +1203,10 @@
         <v>4.12</v>
       </c>
       <c r="C40">
-        <v>4.3</v>
+        <v>5.15</v>
       </c>
       <c r="D40">
-        <v>4.34</v>
+        <v>24.89</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1231,10 +1231,10 @@
         <v>2.21</v>
       </c>
       <c r="C42">
-        <v>2.55</v>
+        <v>2.48</v>
       </c>
       <c r="D42">
-        <v>15.12</v>
+        <v>11.79</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1245,10 +1245,10 @@
         <v>32.85</v>
       </c>
       <c r="C43">
-        <v>32.3</v>
+        <v>32.73</v>
       </c>
       <c r="D43">
-        <v>-1.67</v>
+        <v>-0.37</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1259,10 +1259,10 @@
         <v>21.22</v>
       </c>
       <c r="C44">
-        <v>21.97</v>
+        <v>21.93</v>
       </c>
       <c r="D44">
-        <v>3.55</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1273,10 +1273,10 @@
         <v>6.04</v>
       </c>
       <c r="C45">
-        <v>7.95</v>
+        <v>7.76</v>
       </c>
       <c r="D45">
-        <v>31.68</v>
+        <v>28.41</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1287,10 +1287,10 @@
         <v>20.74</v>
       </c>
       <c r="C46">
-        <v>24.17</v>
+        <v>24.37</v>
       </c>
       <c r="D46">
-        <v>16.56</v>
+        <v>17.49</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1301,10 +1301,10 @@
         <v>20.74</v>
       </c>
       <c r="C47">
-        <v>17.03</v>
+        <v>18.75</v>
       </c>
       <c r="D47">
-        <v>-17.87</v>
+        <v>-9.57</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1315,10 +1315,10 @@
         <v>1.5</v>
       </c>
       <c r="C48">
-        <v>1.68</v>
+        <v>1.8</v>
       </c>
       <c r="D48">
-        <v>12.33</v>
+        <v>19.84</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1329,10 +1329,10 @@
         <v>3.7</v>
       </c>
       <c r="C49">
-        <v>3.88</v>
+        <v>4.01</v>
       </c>
       <c r="D49">
-        <v>4.99</v>
+        <v>8.49</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1343,10 +1343,10 @@
         <v>14.73</v>
       </c>
       <c r="C50">
-        <v>16.3</v>
+        <v>16.47</v>
       </c>
       <c r="D50">
-        <v>10.61</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1371,10 +1371,10 @@
         <v>5.63</v>
       </c>
       <c r="C52">
-        <v>7.1</v>
+        <v>6.82</v>
       </c>
       <c r="D52">
-        <v>26.1</v>
+        <v>21.02</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1385,10 +1385,10 @@
         <v>9.359999999999999</v>
       </c>
       <c r="C53">
-        <v>9.710000000000001</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="D53">
-        <v>3.69</v>
+        <v>5.45</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1399,10 +1399,10 @@
         <v>8.99</v>
       </c>
       <c r="C54">
-        <v>9.57</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="D54">
-        <v>6.47</v>
+        <v>9.73</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1413,10 +1413,10 @@
         <v>34.55</v>
       </c>
       <c r="C55">
-        <v>34.75</v>
+        <v>34.56</v>
       </c>
       <c r="D55">
-        <v>0.57</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1427,10 +1427,10 @@
         <v>3.62</v>
       </c>
       <c r="C56">
-        <v>3.9</v>
+        <v>4.03</v>
       </c>
       <c r="D56">
-        <v>7.89</v>
+        <v>11.46</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1441,10 +1441,10 @@
         <v>11.28</v>
       </c>
       <c r="C57">
-        <v>11.16</v>
+        <v>10.67</v>
       </c>
       <c r="D57">
-        <v>-1.07</v>
+        <v>-5.38</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1455,10 +1455,10 @@
         <v>13.78</v>
       </c>
       <c r="C58">
-        <v>15.17</v>
+        <v>14.82</v>
       </c>
       <c r="D58">
-        <v>10.07</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1469,10 +1469,10 @@
         <v>4.65</v>
       </c>
       <c r="C59">
-        <v>4.62</v>
+        <v>4.78</v>
       </c>
       <c r="D59">
-        <v>-0.57</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1483,10 +1483,10 @@
         <v>5.65</v>
       </c>
       <c r="C60">
-        <v>5.23</v>
+        <v>5.65</v>
       </c>
       <c r="D60">
-        <v>-7.51</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1497,10 +1497,10 @@
         <v>5.3</v>
       </c>
       <c r="C61">
-        <v>5.68</v>
+        <v>4.89</v>
       </c>
       <c r="D61">
-        <v>7.14</v>
+        <v>-7.66</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1511,10 +1511,10 @@
         <v>5.57</v>
       </c>
       <c r="C62">
-        <v>5.07</v>
+        <v>5.01</v>
       </c>
       <c r="D62">
-        <v>-8.960000000000001</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1525,10 +1525,10 @@
         <v>4.75</v>
       </c>
       <c r="C63">
-        <v>4.73</v>
+        <v>4.63</v>
       </c>
       <c r="D63">
-        <v>-0.43</v>
+        <v>-2.66</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1542,7 +1542,7 @@
         <v>3.08</v>
       </c>
       <c r="D64">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1553,10 +1553,10 @@
         <v>7.95</v>
       </c>
       <c r="C65">
-        <v>11.3</v>
+        <v>10.41</v>
       </c>
       <c r="D65">
-        <v>42.2</v>
+        <v>30.92</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1567,10 +1567,10 @@
         <v>2.12</v>
       </c>
       <c r="C66">
-        <v>2.25</v>
+        <v>2.36</v>
       </c>
       <c r="D66">
-        <v>6.17</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1581,10 +1581,10 @@
         <v>3.67</v>
       </c>
       <c r="C67">
-        <v>3.72</v>
+        <v>3.48</v>
       </c>
       <c r="D67">
-        <v>1.48</v>
+        <v>-5.22</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1595,10 +1595,10 @@
         <v>22.51</v>
       </c>
       <c r="C68">
-        <v>20.29</v>
+        <v>20.24</v>
       </c>
       <c r="D68">
-        <v>-9.83</v>
+        <v>-10.05</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1609,10 +1609,10 @@
         <v>52.61</v>
       </c>
       <c r="C69">
-        <v>51.38</v>
+        <v>53.64</v>
       </c>
       <c r="D69">
-        <v>-2.33</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1623,10 +1623,10 @@
         <v>11.7</v>
       </c>
       <c r="C70">
-        <v>9.57</v>
+        <v>10.05</v>
       </c>
       <c r="D70">
-        <v>-18.26</v>
+        <v>-14.13</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1637,10 +1637,10 @@
         <v>7.01</v>
       </c>
       <c r="C71">
-        <v>7.85</v>
+        <v>7.89</v>
       </c>
       <c r="D71">
-        <v>12.02</v>
+        <v>12.64</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1651,10 +1651,10 @@
         <v>30.96</v>
       </c>
       <c r="C72">
-        <v>30.36</v>
+        <v>30.87</v>
       </c>
       <c r="D72">
-        <v>-1.94</v>
+        <v>-0.28</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1679,10 +1679,10 @@
         <v>27.48</v>
       </c>
       <c r="C74">
-        <v>39.05</v>
+        <v>36.36</v>
       </c>
       <c r="D74">
-        <v>42.13</v>
+        <v>32.34</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1693,10 +1693,10 @@
         <v>6.52</v>
       </c>
       <c r="C75">
-        <v>7.06</v>
+        <v>7.2</v>
       </c>
       <c r="D75">
-        <v>8.27</v>
+        <v>10.46</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1721,10 +1721,10 @@
         <v>22.21</v>
       </c>
       <c r="C77">
-        <v>43.97</v>
+        <v>42.14</v>
       </c>
       <c r="D77">
-        <v>97.98</v>
+        <v>89.76000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1735,10 +1735,10 @@
         <v>5.88</v>
       </c>
       <c r="C78">
-        <v>6.65</v>
+        <v>6.85</v>
       </c>
       <c r="D78">
-        <v>13.06</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1749,10 +1749,10 @@
         <v>11.19</v>
       </c>
       <c r="C79">
-        <v>7.69</v>
+        <v>7.52</v>
       </c>
       <c r="D79">
-        <v>-31.3</v>
+        <v>-32.81</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1763,10 +1763,10 @@
         <v>18.5</v>
       </c>
       <c r="C80">
-        <v>19.17</v>
+        <v>18.79</v>
       </c>
       <c r="D80">
-        <v>3.6</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1777,10 +1777,10 @@
         <v>13.84</v>
       </c>
       <c r="C81">
-        <v>14.85</v>
+        <v>14.97</v>
       </c>
       <c r="D81">
-        <v>7.3</v>
+        <v>8.140000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1791,10 +1791,10 @@
         <v>10.81</v>
       </c>
       <c r="C82">
-        <v>15.75</v>
+        <v>15.36</v>
       </c>
       <c r="D82">
-        <v>45.7</v>
+        <v>42.08</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1846,10 +1846,10 @@
         <v>4.27</v>
       </c>
       <c r="C2">
-        <v>6.4</v>
+        <v>6.56</v>
       </c>
       <c r="D2">
-        <v>49.79</v>
+        <v>53.65</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1888,10 +1888,10 @@
         <v>5.05</v>
       </c>
       <c r="C5">
-        <v>7.19</v>
+        <v>7.87</v>
       </c>
       <c r="D5">
-        <v>42.41</v>
+        <v>55.96</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1902,10 +1902,10 @@
         <v>2.4</v>
       </c>
       <c r="C6">
-        <v>11.4</v>
+        <v>11.26</v>
       </c>
       <c r="D6">
-        <v>375.76</v>
+        <v>369.88</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1930,10 +1930,10 @@
         <v>7.77</v>
       </c>
       <c r="C8">
-        <v>6.55</v>
+        <v>6.99</v>
       </c>
       <c r="D8">
-        <v>-15.74</v>
+        <v>-10.1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1944,10 +1944,10 @@
         <v>1.7</v>
       </c>
       <c r="C9">
-        <v>5.37</v>
+        <v>5.14</v>
       </c>
       <c r="D9">
-        <v>216.42</v>
+        <v>202.85</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1958,10 +1958,10 @@
         <v>2.73</v>
       </c>
       <c r="C10">
-        <v>3.48</v>
+        <v>2.73</v>
       </c>
       <c r="D10">
-        <v>27.57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1986,10 +1986,10 @@
         <v>1.31</v>
       </c>
       <c r="C12">
-        <v>4.74</v>
+        <v>5.06</v>
       </c>
       <c r="D12">
-        <v>262.94</v>
+        <v>287.32</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2014,10 +2014,10 @@
         <v>3.46</v>
       </c>
       <c r="C14">
-        <v>5.11</v>
+        <v>4.99</v>
       </c>
       <c r="D14">
-        <v>47.88</v>
+        <v>44.34</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2028,10 +2028,10 @@
         <v>7.26</v>
       </c>
       <c r="C15">
-        <v>7.2</v>
+        <v>7.16</v>
       </c>
       <c r="D15">
-        <v>-0.73</v>
+        <v>-1.33</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2070,10 +2070,10 @@
         <v>10.37</v>
       </c>
       <c r="C18">
-        <v>13.98</v>
+        <v>13.56</v>
       </c>
       <c r="D18">
-        <v>34.76</v>
+        <v>30.67</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2084,10 +2084,10 @@
         <v>13.99</v>
       </c>
       <c r="C19">
-        <v>11.4</v>
+        <v>11.48</v>
       </c>
       <c r="D19">
-        <v>-18.48</v>
+        <v>-17.92</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2140,10 +2140,10 @@
         <v>6.68</v>
       </c>
       <c r="C23">
-        <v>8.119999999999999</v>
+        <v>7.48</v>
       </c>
       <c r="D23">
-        <v>21.66</v>
+        <v>11.94</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2168,10 +2168,10 @@
         <v>3.44</v>
       </c>
       <c r="C25">
-        <v>5.16</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>50.05</v>
+        <v>45.25</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2182,10 +2182,10 @@
         <v>8.75</v>
       </c>
       <c r="C26">
-        <v>9.640000000000001</v>
+        <v>9.23</v>
       </c>
       <c r="D26">
-        <v>10.16</v>
+        <v>5.47</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2224,10 +2224,10 @@
         <v>33.87</v>
       </c>
       <c r="C29">
-        <v>38.95</v>
+        <v>38.94</v>
       </c>
       <c r="D29">
-        <v>15</v>
+        <v>14.98</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2238,10 +2238,10 @@
         <v>43.41</v>
       </c>
       <c r="C30">
-        <v>42.62</v>
+        <v>44.28</v>
       </c>
       <c r="D30">
-        <v>-1.83</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2294,10 +2294,10 @@
         <v>15.24</v>
       </c>
       <c r="C34">
-        <v>10.52</v>
+        <v>12.12</v>
       </c>
       <c r="D34">
-        <v>-30.95</v>
+        <v>-20.45</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2308,10 +2308,10 @@
         <v>7.37</v>
       </c>
       <c r="C35">
-        <v>8.06</v>
+        <v>7.69</v>
       </c>
       <c r="D35">
-        <v>9.33</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2336,10 +2336,10 @@
         <v>7.54</v>
       </c>
       <c r="C37">
-        <v>7.36</v>
+        <v>7.54</v>
       </c>
       <c r="D37">
-        <v>-2.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2350,10 +2350,10 @@
         <v>9.83</v>
       </c>
       <c r="C38">
-        <v>10.78</v>
+        <v>9.83</v>
       </c>
       <c r="D38">
-        <v>9.630000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2378,10 +2378,10 @@
         <v>5.78</v>
       </c>
       <c r="C40">
-        <v>4.23</v>
+        <v>4.86</v>
       </c>
       <c r="D40">
-        <v>-26.89</v>
+        <v>-15.91</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2448,10 +2448,10 @@
         <v>5.17</v>
       </c>
       <c r="C45">
-        <v>8.359999999999999</v>
+        <v>8.15</v>
       </c>
       <c r="D45">
-        <v>61.72</v>
+        <v>57.56</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2476,10 +2476,10 @@
         <v>19.14</v>
       </c>
       <c r="C47">
-        <v>16.51</v>
+        <v>17.92</v>
       </c>
       <c r="D47">
-        <v>-13.71</v>
+        <v>-6.36</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2490,10 +2490,10 @@
         <v>1.82</v>
       </c>
       <c r="C48">
-        <v>1.76</v>
+        <v>1.82</v>
       </c>
       <c r="D48">
-        <v>-3.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2504,10 +2504,10 @@
         <v>5.22</v>
       </c>
       <c r="C49">
-        <v>3.44</v>
+        <v>3.4</v>
       </c>
       <c r="D49">
-        <v>-34.08</v>
+        <v>-34.87</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2546,10 +2546,10 @@
         <v>12.36</v>
       </c>
       <c r="C52">
-        <v>6.86</v>
+        <v>6.64</v>
       </c>
       <c r="D52">
-        <v>-44.5</v>
+        <v>-46.3</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2560,10 +2560,10 @@
         <v>10.28</v>
       </c>
       <c r="C53">
-        <v>9.92</v>
+        <v>9.77</v>
       </c>
       <c r="D53">
-        <v>-3.48</v>
+        <v>-4.9</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2574,10 +2574,10 @@
         <v>7.66</v>
       </c>
       <c r="C54">
-        <v>8.789999999999999</v>
+        <v>9.65</v>
       </c>
       <c r="D54">
-        <v>14.81</v>
+        <v>26.1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2588,10 +2588,10 @@
         <v>26.25</v>
       </c>
       <c r="C55">
-        <v>28.88</v>
+        <v>30.77</v>
       </c>
       <c r="D55">
-        <v>10.04</v>
+        <v>17.25</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2602,10 +2602,10 @@
         <v>3.4</v>
       </c>
       <c r="C56">
-        <v>3.67</v>
+        <v>4.12</v>
       </c>
       <c r="D56">
-        <v>7.85</v>
+        <v>21.24</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2616,10 +2616,10 @@
         <v>9.58</v>
       </c>
       <c r="C57">
-        <v>12.34</v>
+        <v>11.64</v>
       </c>
       <c r="D57">
-        <v>28.78</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2630,10 +2630,10 @@
         <v>13.9</v>
       </c>
       <c r="C58">
-        <v>15.35</v>
+        <v>14.85</v>
       </c>
       <c r="D58">
-        <v>10.41</v>
+        <v>6.85</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2644,10 +2644,10 @@
         <v>4.37</v>
       </c>
       <c r="C59">
-        <v>4.58</v>
+        <v>4.73</v>
       </c>
       <c r="D59">
-        <v>4.81</v>
+        <v>8.369999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2658,10 +2658,10 @@
         <v>3.96</v>
       </c>
       <c r="C60">
-        <v>5.12</v>
+        <v>5.39</v>
       </c>
       <c r="D60">
-        <v>29.19</v>
+        <v>35.85</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2672,10 +2672,10 @@
         <v>5.66</v>
       </c>
       <c r="C61">
-        <v>4.69</v>
+        <v>4.41</v>
       </c>
       <c r="D61">
-        <v>-17.19</v>
+        <v>-22.15</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2689,7 +2689,7 @@
         <v>4.95</v>
       </c>
       <c r="D62">
-        <v>-19.29</v>
+        <v>-19.26</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2700,10 +2700,10 @@
         <v>4.63</v>
       </c>
       <c r="C63">
-        <v>4.61</v>
+        <v>4.54</v>
       </c>
       <c r="D63">
-        <v>-0.38</v>
+        <v>-2.01</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2714,10 +2714,10 @@
         <v>2.92</v>
       </c>
       <c r="C64">
-        <v>2.79</v>
+        <v>2.8</v>
       </c>
       <c r="D64">
-        <v>-4.52</v>
+        <v>-4.13</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2728,10 +2728,10 @@
         <v>6.77</v>
       </c>
       <c r="C65">
-        <v>10.1</v>
+        <v>8.9</v>
       </c>
       <c r="D65">
-        <v>49.32</v>
+        <v>31.59</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2742,10 +2742,10 @@
         <v>2.44</v>
       </c>
       <c r="C66">
-        <v>1.51</v>
+        <v>1.82</v>
       </c>
       <c r="D66">
-        <v>-38.14</v>
+        <v>-25.57</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2756,10 +2756,10 @@
         <v>3.8</v>
       </c>
       <c r="C67">
-        <v>2.91</v>
+        <v>2.66</v>
       </c>
       <c r="D67">
-        <v>-23.26</v>
+        <v>-29.98</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2784,10 +2784,10 @@
         <v>43.55</v>
       </c>
       <c r="C69">
-        <v>50.98</v>
+        <v>54.42</v>
       </c>
       <c r="D69">
-        <v>17.07</v>
+        <v>24.96</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2826,10 +2826,10 @@
         <v>32.9</v>
       </c>
       <c r="C72">
-        <v>29.15</v>
+        <v>28.87</v>
       </c>
       <c r="D72">
-        <v>-11.4</v>
+        <v>-12.24</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2854,10 +2854,10 @@
         <v>37.52</v>
       </c>
       <c r="C74">
-        <v>39.8</v>
+        <v>36.61</v>
       </c>
       <c r="D74">
-        <v>6.1</v>
+        <v>-2.42</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2868,10 +2868,10 @@
         <v>6.33</v>
       </c>
       <c r="C75">
-        <v>6.36</v>
+        <v>6.99</v>
       </c>
       <c r="D75">
-        <v>0.5</v>
+        <v>10.37</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2896,10 +2896,10 @@
         <v>59.48</v>
       </c>
       <c r="C77">
-        <v>41.14</v>
+        <v>42.19</v>
       </c>
       <c r="D77">
-        <v>-30.84</v>
+        <v>-29.07</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2910,10 +2910,10 @@
         <v>6.85</v>
       </c>
       <c r="C78">
-        <v>6.6</v>
+        <v>6.89</v>
       </c>
       <c r="D78">
-        <v>-3.56</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2924,10 +2924,10 @@
         <v>5.91</v>
       </c>
       <c r="C79">
-        <v>7.95</v>
+        <v>7.68</v>
       </c>
       <c r="D79">
-        <v>34.49</v>
+        <v>29.97</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2938,10 +2938,10 @@
         <v>16.88</v>
       </c>
       <c r="C80">
-        <v>19.64</v>
+        <v>19.14</v>
       </c>
       <c r="D80">
-        <v>16.31</v>
+        <v>13.36</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2952,10 +2952,10 @@
         <v>14.63</v>
       </c>
       <c r="C81">
-        <v>14.7</v>
+        <v>14.97</v>
       </c>
       <c r="D81">
-        <v>0.5</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2966,10 +2966,10 @@
         <v>9.210000000000001</v>
       </c>
       <c r="C82">
-        <v>15.71</v>
+        <v>14.92</v>
       </c>
       <c r="D82">
-        <v>70.53</v>
+        <v>61.97</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -3132,7 +3132,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>13.3</v>
+        <v>13.35</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3140,7 +3140,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>13.18</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3148,7 +3148,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>13.39</v>
+        <v>13.49</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3156,7 +3156,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>12.89</v>
+        <v>12.85</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3164,7 +3164,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>13.51</v>
+        <v>13.49</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3172,7 +3172,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>12.91</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3180,7 +3180,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>13.25</v>
+        <v>13.24</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3188,7 +3188,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>12.81</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3196,7 +3196,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>13.19</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3204,7 +3204,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>12.93</v>
+        <v>12.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pipeline outputs, model scripts, and training results
- Updated SSP2-4.5 and SSP5-8.5 predictions and summaries
- Added SHAP analysis results for both scenarios
- Updated model training scripts and visualization
- Added normalized metrics plots and CV test metrics
</commit_message>
<xml_diff>
--- a/Pipeline/SSP2-4.5/banana_yield_analysis.xlsx
+++ b/Pipeline/SSP2-4.5/banana_yield_analysis.xlsx
@@ -671,10 +671,10 @@
         <v>7.46</v>
       </c>
       <c r="C2">
-        <v>7.29</v>
+        <v>6.54</v>
       </c>
       <c r="D2">
-        <v>-2.24</v>
+        <v>-12.33</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -685,10 +685,10 @@
         <v>11.8</v>
       </c>
       <c r="C3">
-        <v>13.84</v>
+        <v>15.76</v>
       </c>
       <c r="D3">
-        <v>17.32</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -699,10 +699,10 @@
         <v>6.53</v>
       </c>
       <c r="C4">
-        <v>7.56</v>
+        <v>7.77</v>
       </c>
       <c r="D4">
-        <v>15.66</v>
+        <v>18.85</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -713,10 +713,10 @@
         <v>6.79</v>
       </c>
       <c r="C5">
-        <v>7.27</v>
+        <v>6.24</v>
       </c>
       <c r="D5">
-        <v>7.06</v>
+        <v>-8.130000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -727,10 +727,10 @@
         <v>15.86</v>
       </c>
       <c r="C6">
-        <v>10.97</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="D6">
-        <v>-30.82</v>
+        <v>-49.31</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -741,10 +741,10 @@
         <v>10.96</v>
       </c>
       <c r="C7">
-        <v>9.220000000000001</v>
+        <v>10.08</v>
       </c>
       <c r="D7">
-        <v>-15.86</v>
+        <v>-8.02</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -755,10 +755,10 @@
         <v>6.76</v>
       </c>
       <c r="C8">
-        <v>7.69</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="D8">
-        <v>13.77</v>
+        <v>22.69</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -768,12 +768,6 @@
       <c r="B9">
         <v>3.91</v>
       </c>
-      <c r="C9">
-        <v>4.42</v>
-      </c>
-      <c r="D9">
-        <v>13.01</v>
-      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
@@ -783,10 +777,10 @@
         <v>3.11</v>
       </c>
       <c r="C10">
-        <v>3.18</v>
+        <v>8.08</v>
       </c>
       <c r="D10">
-        <v>2.15</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -797,10 +791,10 @@
         <v>5.66</v>
       </c>
       <c r="C11">
-        <v>6.42</v>
+        <v>5.58</v>
       </c>
       <c r="D11">
-        <v>13.38</v>
+        <v>-1.35</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -811,10 +805,10 @@
         <v>2.95</v>
       </c>
       <c r="C12">
-        <v>5.87</v>
+        <v>2.39</v>
       </c>
       <c r="D12">
-        <v>99.2</v>
+        <v>-18.76</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -825,10 +819,10 @@
         <v>5.84</v>
       </c>
       <c r="C13">
-        <v>4.49</v>
+        <v>6.17</v>
       </c>
       <c r="D13">
-        <v>-23.07</v>
+        <v>5.69</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -839,10 +833,10 @@
         <v>6.66</v>
       </c>
       <c r="C14">
-        <v>5.1</v>
+        <v>6.33</v>
       </c>
       <c r="D14">
-        <v>-23.43</v>
+        <v>-4.98</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -853,10 +847,10 @@
         <v>8.76</v>
       </c>
       <c r="C15">
-        <v>9.210000000000001</v>
+        <v>7.3</v>
       </c>
       <c r="D15">
-        <v>5.14</v>
+        <v>-16.62</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -867,10 +861,10 @@
         <v>12.01</v>
       </c>
       <c r="C16">
-        <v>14.5</v>
+        <v>13.05</v>
       </c>
       <c r="D16">
-        <v>20.75</v>
+        <v>8.67</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -881,10 +875,10 @@
         <v>61.85</v>
       </c>
       <c r="C17">
-        <v>57.66</v>
+        <v>55.88</v>
       </c>
       <c r="D17">
-        <v>-6.77</v>
+        <v>-9.640000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -895,10 +889,10 @@
         <v>13.07</v>
       </c>
       <c r="C18">
-        <v>13.1</v>
+        <v>11.62</v>
       </c>
       <c r="D18">
-        <v>0.18</v>
+        <v>-11.11</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -908,12 +902,6 @@
       <c r="B19">
         <v>13.86</v>
       </c>
-      <c r="C19">
-        <v>11.98</v>
-      </c>
-      <c r="D19">
-        <v>-13.55</v>
-      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
@@ -923,10 +911,10 @@
         <v>1.88</v>
       </c>
       <c r="C20">
-        <v>2.39</v>
+        <v>2.97</v>
       </c>
       <c r="D20">
-        <v>27.29</v>
+        <v>58.42</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -937,10 +925,10 @@
         <v>3.17</v>
       </c>
       <c r="C21">
-        <v>3.78</v>
+        <v>5.39</v>
       </c>
       <c r="D21">
-        <v>19.26</v>
+        <v>69.73</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -951,10 +939,10 @@
         <v>4.09</v>
       </c>
       <c r="C22">
-        <v>4.89</v>
+        <v>12.65</v>
       </c>
       <c r="D22">
-        <v>19.76</v>
+        <v>209.4</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -965,10 +953,10 @@
         <v>6.85</v>
       </c>
       <c r="C23">
-        <v>8.23</v>
+        <v>7.19</v>
       </c>
       <c r="D23">
-        <v>20.21</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -979,10 +967,10 @@
         <v>2.64</v>
       </c>
       <c r="C24">
-        <v>3.22</v>
+        <v>5.09</v>
       </c>
       <c r="D24">
-        <v>21.91</v>
+        <v>92.94</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -993,10 +981,10 @@
         <v>5.68</v>
       </c>
       <c r="C25">
-        <v>5.46</v>
+        <v>5.58</v>
       </c>
       <c r="D25">
-        <v>-3.92</v>
+        <v>-1.68</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1007,10 +995,10 @@
         <v>8.33</v>
       </c>
       <c r="C26">
-        <v>9.220000000000001</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="D26">
-        <v>10.75</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1021,10 +1009,10 @@
         <v>37.95</v>
       </c>
       <c r="C27">
-        <v>38.79</v>
+        <v>36.82</v>
       </c>
       <c r="D27">
-        <v>2.21</v>
+        <v>-2.97</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1035,10 +1023,10 @@
         <v>15.45</v>
       </c>
       <c r="C28">
-        <v>16.95</v>
+        <v>16.26</v>
       </c>
       <c r="D28">
-        <v>9.699999999999999</v>
+        <v>5.23</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1049,10 +1037,10 @@
         <v>42</v>
       </c>
       <c r="C29">
-        <v>37.8</v>
+        <v>34.35</v>
       </c>
       <c r="D29">
-        <v>-10</v>
+        <v>-18.22</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1063,10 +1051,10 @@
         <v>43.63</v>
       </c>
       <c r="C30">
-        <v>43.74</v>
+        <v>38.87</v>
       </c>
       <c r="D30">
-        <v>0.25</v>
+        <v>-10.91</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1077,10 +1065,10 @@
         <v>38.75</v>
       </c>
       <c r="C31">
-        <v>41.4</v>
+        <v>36.63</v>
       </c>
       <c r="D31">
-        <v>6.84</v>
+        <v>-5.46</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1091,10 +1079,10 @@
         <v>3.08</v>
       </c>
       <c r="C32">
-        <v>5.33</v>
+        <v>7.4</v>
       </c>
       <c r="D32">
-        <v>73.03</v>
+        <v>140.3</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1105,10 +1093,10 @@
         <v>2.58</v>
       </c>
       <c r="C33">
-        <v>3.98</v>
+        <v>3.67</v>
       </c>
       <c r="D33">
-        <v>54.11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1119,10 +1107,10 @@
         <v>11.73</v>
       </c>
       <c r="C34">
-        <v>11.8</v>
+        <v>10.52</v>
       </c>
       <c r="D34">
-        <v>0.59</v>
+        <v>-10.33</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1133,10 +1121,10 @@
         <v>7.4</v>
       </c>
       <c r="C35">
-        <v>7.83</v>
+        <v>7.78</v>
       </c>
       <c r="D35">
-        <v>5.77</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1147,10 +1135,10 @@
         <v>6.26</v>
       </c>
       <c r="C36">
-        <v>6.49</v>
+        <v>8.26</v>
       </c>
       <c r="D36">
-        <v>3.72</v>
+        <v>32.01</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1161,10 +1149,10 @@
         <v>6.67</v>
       </c>
       <c r="C37">
-        <v>7.54</v>
+        <v>7.08</v>
       </c>
       <c r="D37">
-        <v>13.09</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1175,10 +1163,10 @@
         <v>9.93</v>
       </c>
       <c r="C38">
-        <v>10.08</v>
+        <v>8.73</v>
       </c>
       <c r="D38">
-        <v>1.5</v>
+        <v>-12.17</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1189,10 +1177,10 @@
         <v>16.22</v>
       </c>
       <c r="C39">
-        <v>12.72</v>
+        <v>13.37</v>
       </c>
       <c r="D39">
-        <v>-21.55</v>
+        <v>-17.54</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1203,10 +1191,10 @@
         <v>4.12</v>
       </c>
       <c r="C40">
-        <v>5.15</v>
+        <v>5.9</v>
       </c>
       <c r="D40">
-        <v>24.89</v>
+        <v>43.21</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1217,10 +1205,10 @@
         <v>6.55</v>
       </c>
       <c r="C41">
-        <v>7.06</v>
+        <v>6.45</v>
       </c>
       <c r="D41">
-        <v>7.68</v>
+        <v>-1.53</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1231,10 +1219,10 @@
         <v>2.21</v>
       </c>
       <c r="C42">
-        <v>2.48</v>
+        <v>5.16</v>
       </c>
       <c r="D42">
-        <v>11.79</v>
+        <v>132.93</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1245,10 +1233,10 @@
         <v>32.85</v>
       </c>
       <c r="C43">
-        <v>32.73</v>
+        <v>21.47</v>
       </c>
       <c r="D43">
-        <v>-0.37</v>
+        <v>-34.62</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1259,10 +1247,10 @@
         <v>21.22</v>
       </c>
       <c r="C44">
-        <v>21.93</v>
+        <v>21.35</v>
       </c>
       <c r="D44">
-        <v>3.36</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1273,10 +1261,10 @@
         <v>6.04</v>
       </c>
       <c r="C45">
-        <v>7.76</v>
+        <v>7.11</v>
       </c>
       <c r="D45">
-        <v>28.41</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1287,10 +1275,10 @@
         <v>20.74</v>
       </c>
       <c r="C46">
-        <v>24.37</v>
+        <v>17.54</v>
       </c>
       <c r="D46">
-        <v>17.49</v>
+        <v>-15.43</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1301,10 +1289,10 @@
         <v>20.74</v>
       </c>
       <c r="C47">
-        <v>18.75</v>
+        <v>19.01</v>
       </c>
       <c r="D47">
-        <v>-9.57</v>
+        <v>-8.32</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1315,10 +1303,10 @@
         <v>1.5</v>
       </c>
       <c r="C48">
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="D48">
-        <v>19.84</v>
+        <v>140.39</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1329,10 +1317,10 @@
         <v>3.7</v>
       </c>
       <c r="C49">
-        <v>4.01</v>
+        <v>3.7</v>
       </c>
       <c r="D49">
-        <v>8.49</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1343,10 +1331,10 @@
         <v>14.73</v>
       </c>
       <c r="C50">
-        <v>16.47</v>
+        <v>12.87</v>
       </c>
       <c r="D50">
-        <v>11.8</v>
+        <v>-12.67</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1357,10 +1345,10 @@
         <v>12.58</v>
       </c>
       <c r="C51">
-        <v>13.69</v>
+        <v>11.8</v>
       </c>
       <c r="D51">
-        <v>8.869999999999999</v>
+        <v>-6.15</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1371,10 +1359,10 @@
         <v>5.63</v>
       </c>
       <c r="C52">
-        <v>6.82</v>
+        <v>6.25</v>
       </c>
       <c r="D52">
-        <v>21.02</v>
+        <v>10.99</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1385,10 +1373,10 @@
         <v>9.359999999999999</v>
       </c>
       <c r="C53">
-        <v>9.880000000000001</v>
+        <v>9.65</v>
       </c>
       <c r="D53">
-        <v>5.45</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1399,10 +1387,10 @@
         <v>8.99</v>
       </c>
       <c r="C54">
-        <v>9.869999999999999</v>
+        <v>10.19</v>
       </c>
       <c r="D54">
-        <v>9.73</v>
+        <v>13.37</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1413,10 +1401,10 @@
         <v>34.55</v>
       </c>
       <c r="C55">
-        <v>34.56</v>
+        <v>25.17</v>
       </c>
       <c r="D55">
-        <v>0.03</v>
+        <v>-27.17</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1427,10 +1415,10 @@
         <v>3.62</v>
       </c>
       <c r="C56">
-        <v>4.03</v>
+        <v>7.29</v>
       </c>
       <c r="D56">
-        <v>11.46</v>
+        <v>101.52</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1441,10 +1429,10 @@
         <v>11.28</v>
       </c>
       <c r="C57">
-        <v>10.67</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="D57">
-        <v>-5.38</v>
+        <v>-12.6</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1455,10 +1443,10 @@
         <v>13.78</v>
       </c>
       <c r="C58">
-        <v>14.82</v>
+        <v>14.45</v>
       </c>
       <c r="D58">
-        <v>7.5</v>
+        <v>4.82</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1469,10 +1457,10 @@
         <v>4.65</v>
       </c>
       <c r="C59">
-        <v>4.78</v>
+        <v>5.57</v>
       </c>
       <c r="D59">
-        <v>2.73</v>
+        <v>19.79</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1483,10 +1471,10 @@
         <v>5.65</v>
       </c>
       <c r="C60">
-        <v>5.65</v>
+        <v>4.78</v>
       </c>
       <c r="D60">
-        <v>-0.03</v>
+        <v>-15.42</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1497,10 +1485,10 @@
         <v>5.3</v>
       </c>
       <c r="C61">
-        <v>4.89</v>
+        <v>5.02</v>
       </c>
       <c r="D61">
-        <v>-7.66</v>
+        <v>-5.29</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1511,10 +1499,10 @@
         <v>5.57</v>
       </c>
       <c r="C62">
-        <v>5.01</v>
+        <v>6.16</v>
       </c>
       <c r="D62">
-        <v>-10</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1525,10 +1513,10 @@
         <v>4.75</v>
       </c>
       <c r="C63">
-        <v>4.63</v>
+        <v>4.97</v>
       </c>
       <c r="D63">
-        <v>-2.66</v>
+        <v>4.61</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1539,10 +1527,10 @@
         <v>3.08</v>
       </c>
       <c r="C64">
-        <v>3.08</v>
+        <v>3.77</v>
       </c>
       <c r="D64">
-        <v>0.07000000000000001</v>
+        <v>22.46</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1553,10 +1541,10 @@
         <v>7.95</v>
       </c>
       <c r="C65">
-        <v>10.41</v>
+        <v>6.72</v>
       </c>
       <c r="D65">
-        <v>30.92</v>
+        <v>-15.49</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1567,10 +1555,10 @@
         <v>2.12</v>
       </c>
       <c r="C66">
-        <v>2.36</v>
+        <v>4.29</v>
       </c>
       <c r="D66">
-        <v>11.11</v>
+        <v>102.08</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1581,10 +1569,10 @@
         <v>3.67</v>
       </c>
       <c r="C67">
-        <v>3.48</v>
+        <v>5.58</v>
       </c>
       <c r="D67">
-        <v>-5.22</v>
+        <v>52.09</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1595,10 +1583,10 @@
         <v>22.51</v>
       </c>
       <c r="C68">
-        <v>20.24</v>
+        <v>12.99</v>
       </c>
       <c r="D68">
-        <v>-10.05</v>
+        <v>-42.27</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1609,10 +1597,10 @@
         <v>52.61</v>
       </c>
       <c r="C69">
-        <v>53.64</v>
+        <v>38.01</v>
       </c>
       <c r="D69">
-        <v>1.97</v>
+        <v>-27.75</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1623,10 +1611,10 @@
         <v>11.7</v>
       </c>
       <c r="C70">
-        <v>10.05</v>
+        <v>11.96</v>
       </c>
       <c r="D70">
-        <v>-14.13</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1637,10 +1625,10 @@
         <v>7.01</v>
       </c>
       <c r="C71">
-        <v>7.89</v>
+        <v>6.85</v>
       </c>
       <c r="D71">
-        <v>12.64</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1651,10 +1639,10 @@
         <v>30.96</v>
       </c>
       <c r="C72">
-        <v>30.87</v>
+        <v>30.73</v>
       </c>
       <c r="D72">
-        <v>-0.28</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1665,10 +1653,10 @@
         <v>6.49</v>
       </c>
       <c r="C73">
-        <v>7.47</v>
+        <v>7.16</v>
       </c>
       <c r="D73">
-        <v>15.02</v>
+        <v>10.33</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1679,10 +1667,10 @@
         <v>27.48</v>
       </c>
       <c r="C74">
-        <v>36.36</v>
+        <v>32.69</v>
       </c>
       <c r="D74">
-        <v>32.34</v>
+        <v>18.96</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1693,10 +1681,10 @@
         <v>6.52</v>
       </c>
       <c r="C75">
-        <v>7.2</v>
+        <v>7.02</v>
       </c>
       <c r="D75">
-        <v>10.46</v>
+        <v>7.74</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1707,10 +1695,10 @@
         <v>4.51</v>
       </c>
       <c r="C76">
-        <v>9.09</v>
+        <v>6.2</v>
       </c>
       <c r="D76">
-        <v>101.6</v>
+        <v>37.65</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1721,10 +1709,10 @@
         <v>22.21</v>
       </c>
       <c r="C77">
-        <v>42.14</v>
+        <v>24.29</v>
       </c>
       <c r="D77">
-        <v>89.76000000000001</v>
+        <v>9.369999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1735,10 +1723,10 @@
         <v>5.88</v>
       </c>
       <c r="C78">
-        <v>6.85</v>
+        <v>6.88</v>
       </c>
       <c r="D78">
-        <v>16.5</v>
+        <v>17.06</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1748,12 +1736,6 @@
       <c r="B79">
         <v>11.19</v>
       </c>
-      <c r="C79">
-        <v>7.52</v>
-      </c>
-      <c r="D79">
-        <v>-32.81</v>
-      </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
@@ -1763,10 +1745,10 @@
         <v>18.5</v>
       </c>
       <c r="C80">
-        <v>18.79</v>
+        <v>17.57</v>
       </c>
       <c r="D80">
-        <v>1.53</v>
+        <v>-5.03</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1777,10 +1759,10 @@
         <v>13.84</v>
       </c>
       <c r="C81">
-        <v>14.97</v>
+        <v>10.73</v>
       </c>
       <c r="D81">
-        <v>8.140000000000001</v>
+        <v>-22.44</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1791,10 +1773,10 @@
         <v>10.81</v>
       </c>
       <c r="C82">
-        <v>15.36</v>
+        <v>10.8</v>
       </c>
       <c r="D82">
-        <v>42.08</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1805,10 +1787,10 @@
         <v>12.83</v>
       </c>
       <c r="C83">
-        <v>17.38</v>
+        <v>14.31</v>
       </c>
       <c r="D83">
-        <v>35.46</v>
+        <v>11.51</v>
       </c>
     </row>
   </sheetData>
@@ -1846,10 +1828,10 @@
         <v>4.27</v>
       </c>
       <c r="C2">
-        <v>6.56</v>
+        <v>7.42</v>
       </c>
       <c r="D2">
-        <v>53.65</v>
+        <v>73.64</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1860,10 +1842,10 @@
         <v>10.98</v>
       </c>
       <c r="C3">
-        <v>13.84</v>
+        <v>18.31</v>
       </c>
       <c r="D3">
-        <v>26.03</v>
+        <v>66.76000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1874,10 +1856,10 @@
         <v>5.68</v>
       </c>
       <c r="C4">
-        <v>7.56</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="D4">
-        <v>32.97</v>
+        <v>52.04</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1888,10 +1870,10 @@
         <v>5.05</v>
       </c>
       <c r="C5">
-        <v>7.87</v>
+        <v>5.99</v>
       </c>
       <c r="D5">
-        <v>55.96</v>
+        <v>18.67</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1902,10 +1884,10 @@
         <v>2.4</v>
       </c>
       <c r="C6">
-        <v>11.26</v>
+        <v>6.85</v>
       </c>
       <c r="D6">
-        <v>369.88</v>
+        <v>185.97</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1916,10 +1898,10 @@
         <v>11.28</v>
       </c>
       <c r="C7">
-        <v>9.220000000000001</v>
+        <v>10.51</v>
       </c>
       <c r="D7">
-        <v>-18.26</v>
+        <v>-6.85</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1930,10 +1912,10 @@
         <v>7.77</v>
       </c>
       <c r="C8">
-        <v>6.99</v>
+        <v>7.61</v>
       </c>
       <c r="D8">
-        <v>-10.1</v>
+        <v>-2.12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1943,12 +1925,6 @@
       <c r="B9">
         <v>1.7</v>
       </c>
-      <c r="C9">
-        <v>5.14</v>
-      </c>
-      <c r="D9">
-        <v>202.85</v>
-      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
@@ -1958,10 +1934,10 @@
         <v>2.73</v>
       </c>
       <c r="C10">
-        <v>2.73</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>200.86</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1972,10 +1948,10 @@
         <v>5.56</v>
       </c>
       <c r="C11">
-        <v>6.56</v>
+        <v>6.89</v>
       </c>
       <c r="D11">
-        <v>18.09</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1986,10 +1962,10 @@
         <v>1.31</v>
       </c>
       <c r="C12">
-        <v>5.06</v>
+        <v>3.25</v>
       </c>
       <c r="D12">
-        <v>287.32</v>
+        <v>149.28</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2000,10 +1976,10 @@
         <v>5.12</v>
       </c>
       <c r="C13">
-        <v>4.49</v>
+        <v>5.81</v>
       </c>
       <c r="D13">
-        <v>-12.4</v>
+        <v>13.45</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2014,10 +1990,10 @@
         <v>3.46</v>
       </c>
       <c r="C14">
-        <v>4.99</v>
+        <v>6.51</v>
       </c>
       <c r="D14">
-        <v>44.34</v>
+        <v>88.09999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2028,10 +2004,10 @@
         <v>7.26</v>
       </c>
       <c r="C15">
-        <v>7.16</v>
+        <v>7.05</v>
       </c>
       <c r="D15">
-        <v>-1.33</v>
+        <v>-2.83</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2042,10 +2018,10 @@
         <v>7.56</v>
       </c>
       <c r="C16">
-        <v>14.6</v>
+        <v>13.41</v>
       </c>
       <c r="D16">
-        <v>93.23999999999999</v>
+        <v>77.45999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2056,10 +2032,10 @@
         <v>64.16</v>
       </c>
       <c r="C17">
-        <v>56.35</v>
+        <v>57.73</v>
       </c>
       <c r="D17">
-        <v>-12.18</v>
+        <v>-10.03</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2070,10 +2046,10 @@
         <v>10.37</v>
       </c>
       <c r="C18">
-        <v>13.56</v>
+        <v>11.15</v>
       </c>
       <c r="D18">
-        <v>30.67</v>
+        <v>7.45</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2083,12 +2059,6 @@
       <c r="B19">
         <v>13.99</v>
       </c>
-      <c r="C19">
-        <v>11.48</v>
-      </c>
-      <c r="D19">
-        <v>-17.92</v>
-      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
@@ -2098,10 +2068,10 @@
         <v>1.44</v>
       </c>
       <c r="C20">
-        <v>2.48</v>
+        <v>2.86</v>
       </c>
       <c r="D20">
-        <v>71.98</v>
+        <v>98.17</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2112,10 +2082,10 @@
         <v>2.28</v>
       </c>
       <c r="C21">
-        <v>3.79</v>
+        <v>3.83</v>
       </c>
       <c r="D21">
-        <v>65.98999999999999</v>
+        <v>67.81</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2126,10 +2096,10 @@
         <v>3.41</v>
       </c>
       <c r="C22">
-        <v>4.89</v>
+        <v>14.34</v>
       </c>
       <c r="D22">
-        <v>43.61</v>
+        <v>320.78</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2140,10 +2110,10 @@
         <v>6.68</v>
       </c>
       <c r="C23">
-        <v>7.48</v>
+        <v>7.36</v>
       </c>
       <c r="D23">
-        <v>11.94</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2154,10 +2124,10 @@
         <v>1.79</v>
       </c>
       <c r="C24">
-        <v>3.4</v>
+        <v>5.28</v>
       </c>
       <c r="D24">
-        <v>90.31999999999999</v>
+        <v>195.55</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2168,10 +2138,10 @@
         <v>3.44</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>5.82</v>
       </c>
       <c r="D25">
-        <v>45.25</v>
+        <v>69.01000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2182,10 +2152,10 @@
         <v>8.75</v>
       </c>
       <c r="C26">
-        <v>9.23</v>
+        <v>8.41</v>
       </c>
       <c r="D26">
-        <v>5.47</v>
+        <v>-3.89</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2196,10 +2166,10 @@
         <v>37.9</v>
       </c>
       <c r="C27">
-        <v>38.79</v>
+        <v>34.27</v>
       </c>
       <c r="D27">
-        <v>2.33</v>
+        <v>-9.58</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2210,10 +2180,10 @@
         <v>14.91</v>
       </c>
       <c r="C28">
-        <v>17.25</v>
+        <v>13.51</v>
       </c>
       <c r="D28">
-        <v>15.7</v>
+        <v>-9.390000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2224,10 +2194,10 @@
         <v>33.87</v>
       </c>
       <c r="C29">
-        <v>38.94</v>
+        <v>37.7</v>
       </c>
       <c r="D29">
-        <v>14.98</v>
+        <v>11.33</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2238,10 +2208,10 @@
         <v>43.41</v>
       </c>
       <c r="C30">
-        <v>44.28</v>
+        <v>37.44</v>
       </c>
       <c r="D30">
-        <v>2.01</v>
+        <v>-13.75</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2252,10 +2222,10 @@
         <v>37.25</v>
       </c>
       <c r="C31">
-        <v>41.4</v>
+        <v>38.31</v>
       </c>
       <c r="D31">
-        <v>11.13</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2266,10 +2236,10 @@
         <v>3.67</v>
       </c>
       <c r="C32">
-        <v>5.33</v>
+        <v>6.14</v>
       </c>
       <c r="D32">
-        <v>45.14</v>
+        <v>67.12</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2280,10 +2250,10 @@
         <v>2.79</v>
       </c>
       <c r="C33">
-        <v>3.98</v>
+        <v>4.25</v>
       </c>
       <c r="D33">
-        <v>42.68</v>
+        <v>52.27</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2294,10 +2264,10 @@
         <v>15.24</v>
       </c>
       <c r="C34">
-        <v>12.12</v>
+        <v>10.71</v>
       </c>
       <c r="D34">
-        <v>-20.45</v>
+        <v>-29.75</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2308,10 +2278,10 @@
         <v>7.37</v>
       </c>
       <c r="C35">
-        <v>7.69</v>
+        <v>9.51</v>
       </c>
       <c r="D35">
-        <v>4.28</v>
+        <v>29.02</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2322,10 +2292,10 @@
         <v>6.75</v>
       </c>
       <c r="C36">
-        <v>7.33</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="D36">
-        <v>8.550000000000001</v>
+        <v>21.65</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2336,10 +2306,10 @@
         <v>7.54</v>
       </c>
       <c r="C37">
-        <v>7.54</v>
+        <v>6.96</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>-7.75</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2350,10 +2320,10 @@
         <v>9.83</v>
       </c>
       <c r="C38">
-        <v>9.83</v>
+        <v>9.52</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>-3.14</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2364,10 +2334,10 @@
         <v>15.02</v>
       </c>
       <c r="C39">
-        <v>12.72</v>
+        <v>12.14</v>
       </c>
       <c r="D39">
-        <v>-15.29</v>
+        <v>-19.19</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2378,10 +2348,10 @@
         <v>5.78</v>
       </c>
       <c r="C40">
-        <v>4.86</v>
+        <v>6.02</v>
       </c>
       <c r="D40">
-        <v>-15.91</v>
+        <v>4.16</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2392,10 +2362,10 @@
         <v>6.4</v>
       </c>
       <c r="C41">
-        <v>7.06</v>
+        <v>6.51</v>
       </c>
       <c r="D41">
-        <v>10.23</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2406,10 +2376,10 @@
         <v>1.72</v>
       </c>
       <c r="C42">
-        <v>2.84</v>
+        <v>5.14</v>
       </c>
       <c r="D42">
-        <v>64.81999999999999</v>
+        <v>198.11</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2420,10 +2390,10 @@
         <v>32.66</v>
       </c>
       <c r="C43">
-        <v>32.3</v>
+        <v>23.46</v>
       </c>
       <c r="D43">
-        <v>-1.11</v>
+        <v>-28.16</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2434,10 +2404,10 @@
         <v>21.38</v>
       </c>
       <c r="C44">
-        <v>21.97</v>
+        <v>23.1</v>
       </c>
       <c r="D44">
-        <v>2.76</v>
+        <v>8.02</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2448,10 +2418,10 @@
         <v>5.17</v>
       </c>
       <c r="C45">
-        <v>8.15</v>
+        <v>8.08</v>
       </c>
       <c r="D45">
-        <v>57.56</v>
+        <v>56.16</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2462,10 +2432,10 @@
         <v>19.14</v>
       </c>
       <c r="C46">
-        <v>24.37</v>
+        <v>18.17</v>
       </c>
       <c r="D46">
-        <v>27.33</v>
+        <v>-5.05</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2476,10 +2446,10 @@
         <v>19.14</v>
       </c>
       <c r="C47">
-        <v>17.92</v>
+        <v>19.49</v>
       </c>
       <c r="D47">
-        <v>-6.36</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2490,10 +2460,10 @@
         <v>1.82</v>
       </c>
       <c r="C48">
-        <v>1.82</v>
+        <v>3.39</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>86.19</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2504,10 +2474,10 @@
         <v>5.22</v>
       </c>
       <c r="C49">
-        <v>3.4</v>
+        <v>3.89</v>
       </c>
       <c r="D49">
-        <v>-34.87</v>
+        <v>-25.54</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2518,10 +2488,10 @@
         <v>14.73</v>
       </c>
       <c r="C50">
-        <v>16.51</v>
+        <v>13.51</v>
       </c>
       <c r="D50">
-        <v>12.06</v>
+        <v>-8.279999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2532,10 +2502,10 @@
         <v>12.27</v>
       </c>
       <c r="C51">
-        <v>13.69</v>
+        <v>13.92</v>
       </c>
       <c r="D51">
-        <v>11.61</v>
+        <v>13.52</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2546,10 +2516,10 @@
         <v>12.36</v>
       </c>
       <c r="C52">
-        <v>6.64</v>
+        <v>5.74</v>
       </c>
       <c r="D52">
-        <v>-46.3</v>
+        <v>-53.55</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2560,10 +2530,10 @@
         <v>10.28</v>
       </c>
       <c r="C53">
-        <v>9.77</v>
+        <v>11.25</v>
       </c>
       <c r="D53">
-        <v>-4.9</v>
+        <v>9.44</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2574,10 +2544,10 @@
         <v>7.66</v>
       </c>
       <c r="C54">
-        <v>9.65</v>
+        <v>12.6</v>
       </c>
       <c r="D54">
-        <v>26.1</v>
+        <v>64.56999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2588,10 +2558,10 @@
         <v>26.25</v>
       </c>
       <c r="C55">
-        <v>30.77</v>
+        <v>25.47</v>
       </c>
       <c r="D55">
-        <v>17.25</v>
+        <v>-2.96</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2602,10 +2572,10 @@
         <v>3.4</v>
       </c>
       <c r="C56">
-        <v>4.12</v>
+        <v>10.45</v>
       </c>
       <c r="D56">
-        <v>21.24</v>
+        <v>207.38</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2616,10 +2586,10 @@
         <v>9.58</v>
       </c>
       <c r="C57">
-        <v>11.64</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="D57">
-        <v>21.5</v>
+        <v>-0.59</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2630,10 +2600,10 @@
         <v>13.9</v>
       </c>
       <c r="C58">
-        <v>14.85</v>
+        <v>17.39</v>
       </c>
       <c r="D58">
-        <v>6.85</v>
+        <v>25.14</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2644,10 +2614,10 @@
         <v>4.37</v>
       </c>
       <c r="C59">
-        <v>4.73</v>
+        <v>5.9</v>
       </c>
       <c r="D59">
-        <v>8.369999999999999</v>
+        <v>35.11</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2661,7 +2631,7 @@
         <v>5.39</v>
       </c>
       <c r="D60">
-        <v>35.85</v>
+        <v>35.96</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2672,10 +2642,10 @@
         <v>5.66</v>
       </c>
       <c r="C61">
-        <v>4.41</v>
+        <v>5.14</v>
       </c>
       <c r="D61">
-        <v>-22.15</v>
+        <v>-9.27</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2686,10 +2656,10 @@
         <v>6.14</v>
       </c>
       <c r="C62">
-        <v>4.95</v>
+        <v>6.27</v>
       </c>
       <c r="D62">
-        <v>-19.26</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2700,10 +2670,10 @@
         <v>4.63</v>
       </c>
       <c r="C63">
-        <v>4.54</v>
+        <v>5.12</v>
       </c>
       <c r="D63">
-        <v>-2.01</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2714,10 +2684,10 @@
         <v>2.92</v>
       </c>
       <c r="C64">
-        <v>2.8</v>
+        <v>3.91</v>
       </c>
       <c r="D64">
-        <v>-4.13</v>
+        <v>33.7</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2728,10 +2698,10 @@
         <v>6.77</v>
       </c>
       <c r="C65">
-        <v>8.9</v>
+        <v>8.27</v>
       </c>
       <c r="D65">
-        <v>31.59</v>
+        <v>22.23</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2742,10 +2712,10 @@
         <v>2.44</v>
       </c>
       <c r="C66">
-        <v>1.82</v>
+        <v>5.1</v>
       </c>
       <c r="D66">
-        <v>-25.57</v>
+        <v>109.12</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2756,10 +2726,10 @@
         <v>3.8</v>
       </c>
       <c r="C67">
-        <v>2.66</v>
+        <v>5.79</v>
       </c>
       <c r="D67">
-        <v>-29.98</v>
+        <v>52.47</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2770,10 +2740,10 @@
         <v>20.01</v>
       </c>
       <c r="C68">
-        <v>19.93</v>
+        <v>10.29</v>
       </c>
       <c r="D68">
-        <v>-0.38</v>
+        <v>-48.55</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2784,10 +2754,10 @@
         <v>43.55</v>
       </c>
       <c r="C69">
-        <v>54.42</v>
+        <v>37.68</v>
       </c>
       <c r="D69">
-        <v>24.96</v>
+        <v>-13.48</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2798,10 +2768,10 @@
         <v>11.63</v>
       </c>
       <c r="C70">
-        <v>8.48</v>
+        <v>15.07</v>
       </c>
       <c r="D70">
-        <v>-27.04</v>
+        <v>29.57</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2812,10 +2782,10 @@
         <v>4.92</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>7.38</v>
       </c>
       <c r="D71">
-        <v>62.59</v>
+        <v>50.01</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2826,10 +2796,10 @@
         <v>32.9</v>
       </c>
       <c r="C72">
-        <v>28.87</v>
+        <v>30.65</v>
       </c>
       <c r="D72">
-        <v>-12.24</v>
+        <v>-6.85</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2840,10 +2810,10 @@
         <v>7.47</v>
       </c>
       <c r="C73">
-        <v>7.47</v>
+        <v>8.32</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>11.47</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2854,10 +2824,10 @@
         <v>37.52</v>
       </c>
       <c r="C74">
-        <v>36.61</v>
+        <v>35.81</v>
       </c>
       <c r="D74">
-        <v>-2.42</v>
+        <v>-4.54</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2868,10 +2838,10 @@
         <v>6.33</v>
       </c>
       <c r="C75">
-        <v>6.99</v>
+        <v>7.25</v>
       </c>
       <c r="D75">
-        <v>10.37</v>
+        <v>14.56</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2882,10 +2852,10 @@
         <v>1.59</v>
       </c>
       <c r="C76">
-        <v>9.09</v>
+        <v>5.59</v>
       </c>
       <c r="D76">
-        <v>469.76</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2896,10 +2866,10 @@
         <v>59.48</v>
       </c>
       <c r="C77">
-        <v>42.19</v>
+        <v>20.29</v>
       </c>
       <c r="D77">
-        <v>-29.07</v>
+        <v>-65.89</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2910,10 +2880,10 @@
         <v>6.85</v>
       </c>
       <c r="C78">
-        <v>6.89</v>
+        <v>6.94</v>
       </c>
       <c r="D78">
-        <v>0.67</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2923,12 +2893,6 @@
       <c r="B79">
         <v>5.91</v>
       </c>
-      <c r="C79">
-        <v>7.68</v>
-      </c>
-      <c r="D79">
-        <v>29.97</v>
-      </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
@@ -2938,10 +2902,10 @@
         <v>16.88</v>
       </c>
       <c r="C80">
-        <v>19.14</v>
+        <v>17.29</v>
       </c>
       <c r="D80">
-        <v>13.36</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2952,10 +2916,10 @@
         <v>14.63</v>
       </c>
       <c r="C81">
-        <v>14.97</v>
+        <v>12.02</v>
       </c>
       <c r="D81">
-        <v>2.29</v>
+        <v>-17.85</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2966,10 +2930,10 @@
         <v>9.210000000000001</v>
       </c>
       <c r="C82">
-        <v>14.92</v>
+        <v>11.49</v>
       </c>
       <c r="D82">
-        <v>61.97</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2980,10 +2944,10 @@
         <v>16.53</v>
       </c>
       <c r="C83">
-        <v>17.38</v>
+        <v>15.56</v>
       </c>
       <c r="D83">
-        <v>5.15</v>
+        <v>-5.84</v>
       </c>
     </row>
   </sheetData>
@@ -3132,7 +3096,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>13.35</v>
+        <v>10.78</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3140,7 +3104,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>13.25</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3148,7 +3112,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>13.49</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3156,7 +3120,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>12.85</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3164,7 +3128,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>13.49</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3172,7 +3136,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>12.86</v>
+        <v>12.48</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3180,7 +3144,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>13.24</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3188,7 +3152,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>12.8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3196,7 +3160,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>13.2</v>
+        <v>13.06</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3204,7 +3168,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>12.98</v>
+        <v>12.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>